<commit_message>
Updated main and xlsx files
</commit_message>
<xml_diff>
--- a/m5out_stats.xlsx
+++ b/m5out_stats.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -896,6 +896,35 @@
         <v>13317.924994</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1657238.437593</v>
+      </c>
+      <c r="C16" t="n">
+        <v>20357.699105</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1636880.738488</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12974.03040366667</v>
+      </c>
+      <c r="F16" t="n">
+        <v>748182.757149</v>
+      </c>
+      <c r="G16" t="n">
+        <v>14232.5759</v>
+      </c>
+      <c r="H16" t="n">
+        <v>733950.18125</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14840.43002133333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated main and xlsx file
</commit_message>
<xml_diff>
--- a/m5out_stats.xlsx
+++ b/m5out_stats.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -954,6 +954,151 @@
         <v>15537.91470366667</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4236727.498161</v>
+      </c>
+      <c r="C18" t="n">
+        <v>21243.694582</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4215483.803579</v>
+      </c>
+      <c r="E18" t="n">
+        <v>13991.442363</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1760426.373385</v>
+      </c>
+      <c r="G18" t="n">
+        <v>14071.290441</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1746355.082944</v>
+      </c>
+      <c r="I18" t="n">
+        <v>15981.531147</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5117794.229655</v>
+      </c>
+      <c r="C19" t="n">
+        <v>21393.73706</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5096400.492595</v>
+      </c>
+      <c r="E19" t="n">
+        <v>14391.29253366667</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2050415.88006</v>
+      </c>
+      <c r="G19" t="n">
+        <v>13914.390853</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2036501.489207</v>
+      </c>
+      <c r="I19" t="n">
+        <v>16453.033397</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5880494.184356</v>
+      </c>
+      <c r="C20" t="n">
+        <v>21702.176071</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5858792.008285</v>
+      </c>
+      <c r="E20" t="n">
+        <v>14916.40278166667</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2266081.715755</v>
+      </c>
+      <c r="G20" t="n">
+        <v>13768.710049</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2252313.005706</v>
+      </c>
+      <c r="I20" t="n">
+        <v>17045.34805033333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6426087.193499</v>
+      </c>
+      <c r="C21" t="n">
+        <v>21818.546042</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6404268.647457</v>
+      </c>
+      <c r="E21" t="n">
+        <v>15350.98245466666</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2395551.12106</v>
+      </c>
+      <c r="G21" t="n">
+        <v>13640.013058</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2381911.108002</v>
+      </c>
+      <c r="I21" t="n">
+        <v>17559.29677233333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6841596.896981</v>
+      </c>
+      <c r="C22" t="n">
+        <v>22087.582224</v>
+      </c>
+      <c r="D22" t="n">
+        <v>6819509.314757</v>
+      </c>
+      <c r="E22" t="n">
+        <v>15900.36611133333</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2470749.551649</v>
+      </c>
+      <c r="G22" t="n">
+        <v>13579.795378</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2457169.756271</v>
+      </c>
+      <c r="I22" t="n">
+        <v>18182.396295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated xlsx files for triba27 and mesh16 and mesh 32
</commit_message>
<xml_diff>
--- a/m5out_stats.xlsx
+++ b/m5out_stats.xlsx
@@ -424,10 +424,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -495,28 +495,28 @@
         <v>0.01</v>
       </c>
       <c r="B2" t="n">
-        <v>5793.051934</v>
+        <v>7173.133838</v>
       </c>
       <c r="C2" t="n">
-        <v>4793.051934</v>
+        <v>6173.133838</v>
       </c>
       <c r="D2" t="n">
         <v>1000</v>
       </c>
       <c r="E2" t="n">
-        <v>4369.380304333333</v>
+        <v>5736.206039333334</v>
       </c>
       <c r="F2" t="n">
-        <v>5834.240506</v>
+        <v>7193.05485</v>
       </c>
       <c r="G2" t="n">
-        <v>4834.240506</v>
+        <v>6193.05485</v>
       </c>
       <c r="H2" t="n">
         <v>1000</v>
       </c>
       <c r="I2" t="n">
-        <v>4836.478388333333</v>
+        <v>6203.567016666668</v>
       </c>
     </row>
     <row r="3">
@@ -524,28 +524,28 @@
         <v>0.03</v>
       </c>
       <c r="B3" t="n">
-        <v>5858.433572</v>
+        <v>7280.891622</v>
       </c>
       <c r="C3" t="n">
-        <v>4858.433572</v>
+        <v>6280.891622</v>
       </c>
       <c r="D3" t="n">
         <v>1000</v>
       </c>
       <c r="E3" t="n">
-        <v>4410.11708</v>
+        <v>5810.779687333333</v>
       </c>
       <c r="F3" t="n">
-        <v>5872.207608</v>
+        <v>7275.870006</v>
       </c>
       <c r="G3" t="n">
-        <v>4872.207608</v>
+        <v>6275.870006</v>
       </c>
       <c r="H3" t="n">
         <v>1000</v>
       </c>
       <c r="I3" t="n">
-        <v>4879.343638666666</v>
+        <v>6286.564092666667</v>
       </c>
     </row>
     <row r="4">
@@ -553,28 +553,28 @@
         <v>0.05</v>
       </c>
       <c r="B4" t="n">
-        <v>5894.277286</v>
+        <v>7341.247585</v>
       </c>
       <c r="C4" t="n">
-        <v>4894.277286</v>
+        <v>6341.247585</v>
       </c>
       <c r="D4" t="n">
         <v>1000</v>
       </c>
       <c r="E4" t="n">
-        <v>4435.926576999999</v>
+        <v>5849.035594333333</v>
       </c>
       <c r="F4" t="n">
-        <v>5903.339804</v>
+        <v>7331.611144</v>
       </c>
       <c r="G4" t="n">
-        <v>4903.339804</v>
+        <v>6331.611144</v>
       </c>
       <c r="H4" t="n">
         <v>1000</v>
       </c>
       <c r="I4" t="n">
-        <v>4912.129360666667</v>
+        <v>6337.965039</v>
       </c>
     </row>
     <row r="5">
@@ -582,28 +582,28 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>6037.336376</v>
+        <v>7595.599797</v>
       </c>
       <c r="C5" t="n">
-        <v>5037.336376</v>
+        <v>6595.586358</v>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>1000.013439</v>
       </c>
       <c r="E5" t="n">
-        <v>4505.116047333334</v>
+        <v>5991.863622</v>
       </c>
       <c r="F5" t="n">
-        <v>6007.613421</v>
+        <v>7541.97308</v>
       </c>
       <c r="G5" t="n">
-        <v>5007.613421</v>
+        <v>6541.96681</v>
       </c>
       <c r="H5" t="n">
-        <v>1000</v>
+        <v>1000.006269</v>
       </c>
       <c r="I5" t="n">
-        <v>5008.411500333334</v>
+        <v>6542.697749</v>
       </c>
     </row>
     <row r="6">
@@ -611,28 +611,28 @@
         <v>0.15</v>
       </c>
       <c r="B6" t="n">
-        <v>6200.236695</v>
+        <v>7966.155545</v>
       </c>
       <c r="C6" t="n">
-        <v>5200.138221</v>
+        <v>6965.985549</v>
       </c>
       <c r="D6" t="n">
-        <v>1000.098474</v>
+        <v>1000.169996</v>
       </c>
       <c r="E6" t="n">
-        <v>4600.728950333333</v>
+        <v>6207.655787666667</v>
       </c>
       <c r="F6" t="n">
-        <v>6146.168682</v>
+        <v>7863.416632</v>
       </c>
       <c r="G6" t="n">
-        <v>5146.122762</v>
+        <v>6863.337247</v>
       </c>
       <c r="H6" t="n">
-        <v>1000.045919</v>
+        <v>1000.079385</v>
       </c>
       <c r="I6" t="n">
-        <v>5147.672062000001</v>
+        <v>6861.860122000001</v>
       </c>
     </row>
     <row r="7">
@@ -640,28 +640,28 @@
         <v>0.2</v>
       </c>
       <c r="B7" t="n">
-        <v>6391.183419</v>
+        <v>8498.084977</v>
       </c>
       <c r="C7" t="n">
-        <v>5390.747154</v>
+        <v>7497.400801</v>
       </c>
       <c r="D7" t="n">
-        <v>1000.436265</v>
+        <v>1000.684176</v>
       </c>
       <c r="E7" t="n">
-        <v>4709.541205</v>
+        <v>6527.372342333333</v>
       </c>
       <c r="F7" t="n">
-        <v>6315.335219</v>
+        <v>8324.692282</v>
       </c>
       <c r="G7" t="n">
-        <v>5315.13181</v>
+        <v>7324.3729</v>
       </c>
       <c r="H7" t="n">
-        <v>1000.20341</v>
+        <v>1000.319382</v>
       </c>
       <c r="I7" t="n">
-        <v>5317.001964333333</v>
+        <v>7323.564589000001</v>
       </c>
     </row>
     <row r="8">
@@ -669,28 +669,28 @@
         <v>0.25</v>
       </c>
       <c r="B8" t="n">
-        <v>6639.648164</v>
+        <v>9442.517527</v>
       </c>
       <c r="C8" t="n">
-        <v>5637.524463</v>
+        <v>8439.661268</v>
       </c>
       <c r="D8" t="n">
-        <v>1002.123702</v>
+        <v>1002.856259</v>
       </c>
       <c r="E8" t="n">
-        <v>4852.334717000001</v>
+        <v>7087.346924333334</v>
       </c>
       <c r="F8" t="n">
-        <v>6529.588937</v>
+        <v>9077.910517</v>
       </c>
       <c r="G8" t="n">
-        <v>5528.600805</v>
+        <v>8076.578393</v>
       </c>
       <c r="H8" t="n">
-        <v>1000.988132</v>
+        <v>1001.332125</v>
       </c>
       <c r="I8" t="n">
-        <v>5535.715037999999</v>
+        <v>8081.934995333334</v>
       </c>
     </row>
     <row r="9">
@@ -698,405 +698,28 @@
         <v>0.3</v>
       </c>
       <c r="B9" t="n">
-        <v>6970.688791</v>
+        <v>11748.808007</v>
       </c>
       <c r="C9" t="n">
-        <v>5965.029461</v>
+        <v>10730.621608</v>
       </c>
       <c r="D9" t="n">
-        <v>1005.65933</v>
+        <v>1018.186398</v>
       </c>
       <c r="E9" t="n">
-        <v>5048.525075</v>
+        <v>8369.032585999999</v>
       </c>
       <c r="F9" t="n">
-        <v>6824.862159</v>
+        <v>10627.947995</v>
       </c>
       <c r="G9" t="n">
-        <v>5822.228288</v>
+        <v>9619.474072999999</v>
       </c>
       <c r="H9" t="n">
-        <v>1002.633871</v>
+        <v>1008.473923</v>
       </c>
       <c r="I9" t="n">
-        <v>5829.845438</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="B10" t="n">
-        <v>7393.831659</v>
-      </c>
-      <c r="C10" t="n">
-        <v>6378.169465</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1015.662194</v>
-      </c>
-      <c r="E10" t="n">
-        <v>5296.928606666667</v>
-      </c>
-      <c r="F10" t="n">
-        <v>7192.569524</v>
-      </c>
-      <c r="G10" t="n">
-        <v>6185.272055</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1007.297469</v>
-      </c>
-      <c r="I10" t="n">
-        <v>6190.386768666666</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="B11" t="n">
-        <v>7964.58162</v>
-      </c>
-      <c r="C11" t="n">
-        <v>6930.080708</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1034.500913</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5629.711921666666</v>
-      </c>
-      <c r="F11" t="n">
-        <v>7672.33402</v>
-      </c>
-      <c r="G11" t="n">
-        <v>6656.247948</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1016.086072</v>
-      </c>
-      <c r="I11" t="n">
-        <v>6660.858432666667</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="B12" t="n">
-        <v>8820.569142</v>
-      </c>
-      <c r="C12" t="n">
-        <v>7737.386025</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1083.183117</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6118.666528000001</v>
-      </c>
-      <c r="F12" t="n">
-        <v>8339.959801999999</v>
-      </c>
-      <c r="G12" t="n">
-        <v>7301.210111</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1038.749691</v>
-      </c>
-      <c r="I12" t="n">
-        <v>7310.521375333333</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B13" t="n">
-        <v>10372.367021</v>
-      </c>
-      <c r="C13" t="n">
-        <v>9110.323339</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1262.043681</v>
-      </c>
-      <c r="E13" t="n">
-        <v>6920.688342333334</v>
-      </c>
-      <c r="F13" t="n">
-        <v>9424.393330999999</v>
-      </c>
-      <c r="G13" t="n">
-        <v>8302.225329000001</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1122.168001</v>
-      </c>
-      <c r="I13" t="n">
-        <v>8307.906024333333</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B14" t="n">
-        <v>14296.654843</v>
-      </c>
-      <c r="C14" t="n">
-        <v>11532.403804</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2764.251039</v>
-      </c>
-      <c r="E14" t="n">
-        <v>8263.872064000001</v>
-      </c>
-      <c r="F14" t="n">
-        <v>11674.589409</v>
-      </c>
-      <c r="G14" t="n">
-        <v>9851.230351</v>
-      </c>
-      <c r="H14" t="n">
-        <v>1823.359058</v>
-      </c>
-      <c r="I14" t="n">
-        <v>9851.823604333333</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="B15" t="n">
-        <v>189857.022604</v>
-      </c>
-      <c r="C15" t="n">
-        <v>17841.143571</v>
-      </c>
-      <c r="D15" t="n">
-        <v>172015.879033</v>
-      </c>
-      <c r="E15" t="n">
-        <v>11520.41209333333</v>
-      </c>
-      <c r="F15" t="n">
-        <v>93783.901664</v>
-      </c>
-      <c r="G15" t="n">
-        <v>13273.507545</v>
-      </c>
-      <c r="H15" t="n">
-        <v>80510.394119</v>
-      </c>
-      <c r="I15" t="n">
-        <v>13317.924994</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1657238.437593</v>
-      </c>
-      <c r="C16" t="n">
-        <v>20357.699105</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1636880.738488</v>
-      </c>
-      <c r="E16" t="n">
-        <v>12974.03040366667</v>
-      </c>
-      <c r="F16" t="n">
-        <v>748182.757149</v>
-      </c>
-      <c r="G16" t="n">
-        <v>14232.5759</v>
-      </c>
-      <c r="H16" t="n">
-        <v>733950.18125</v>
-      </c>
-      <c r="I16" t="n">
-        <v>14840.43002133333</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="B17" t="n">
-        <v>2985065.736644</v>
-      </c>
-      <c r="C17" t="n">
-        <v>21057.645339</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2964008.091305</v>
-      </c>
-      <c r="E17" t="n">
-        <v>13607.360941</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1290516.054363</v>
-      </c>
-      <c r="G17" t="n">
-        <v>14272.357413</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1276243.69695</v>
-      </c>
-      <c r="I17" t="n">
-        <v>15537.91470366667</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B18" t="n">
-        <v>4236727.498161</v>
-      </c>
-      <c r="C18" t="n">
-        <v>21243.694582</v>
-      </c>
-      <c r="D18" t="n">
-        <v>4215483.803579</v>
-      </c>
-      <c r="E18" t="n">
-        <v>13991.442363</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1760426.373385</v>
-      </c>
-      <c r="G18" t="n">
-        <v>14071.290441</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1746355.082944</v>
-      </c>
-      <c r="I18" t="n">
-        <v>15981.531147</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="B19" t="n">
-        <v>5117794.229655</v>
-      </c>
-      <c r="C19" t="n">
-        <v>21393.73706</v>
-      </c>
-      <c r="D19" t="n">
-        <v>5096400.492595</v>
-      </c>
-      <c r="E19" t="n">
-        <v>14391.29253366667</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2050415.88006</v>
-      </c>
-      <c r="G19" t="n">
-        <v>13914.390853</v>
-      </c>
-      <c r="H19" t="n">
-        <v>2036501.489207</v>
-      </c>
-      <c r="I19" t="n">
-        <v>16453.033397</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="B20" t="n">
-        <v>5880494.184356</v>
-      </c>
-      <c r="C20" t="n">
-        <v>21702.176071</v>
-      </c>
-      <c r="D20" t="n">
-        <v>5858792.008285</v>
-      </c>
-      <c r="E20" t="n">
-        <v>14916.40278166667</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2266081.715755</v>
-      </c>
-      <c r="G20" t="n">
-        <v>13768.710049</v>
-      </c>
-      <c r="H20" t="n">
-        <v>2252313.005706</v>
-      </c>
-      <c r="I20" t="n">
-        <v>17045.34805033333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="B21" t="n">
-        <v>6426087.193499</v>
-      </c>
-      <c r="C21" t="n">
-        <v>21818.546042</v>
-      </c>
-      <c r="D21" t="n">
-        <v>6404268.647457</v>
-      </c>
-      <c r="E21" t="n">
-        <v>15350.98245466666</v>
-      </c>
-      <c r="F21" t="n">
-        <v>2395551.12106</v>
-      </c>
-      <c r="G21" t="n">
-        <v>13640.013058</v>
-      </c>
-      <c r="H21" t="n">
-        <v>2381911.108002</v>
-      </c>
-      <c r="I21" t="n">
-        <v>17559.29677233333</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="B22" t="n">
-        <v>6841596.896981</v>
-      </c>
-      <c r="C22" t="n">
-        <v>22087.582224</v>
-      </c>
-      <c r="D22" t="n">
-        <v>6819509.314757</v>
-      </c>
-      <c r="E22" t="n">
-        <v>15900.36611133333</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2470749.551649</v>
-      </c>
-      <c r="G22" t="n">
-        <v>13579.795378</v>
-      </c>
-      <c r="H22" t="n">
-        <v>2457169.756271</v>
-      </c>
-      <c r="I22" t="n">
-        <v>18182.396295</v>
+        <v>9628.793535666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated main and xlsx
</commit_message>
<xml_diff>
--- a/m5out_stats.xlsx
+++ b/m5out_stats.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -925,6 +925,151 @@
         <v>26.749201902</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3911.892387694</v>
+      </c>
+      <c r="C17" t="n">
+        <v>37.487058824</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3874.405328872</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25.440260226</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1585.105019658</v>
+      </c>
+      <c r="G17" t="n">
+        <v>23.140807668</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1561.96421199</v>
+      </c>
+      <c r="I17" t="n">
+        <v>26.67706112333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4041.011614314</v>
+      </c>
+      <c r="C18" t="n">
+        <v>36.964767414</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4004.0468469</v>
+      </c>
+      <c r="E18" t="n">
+        <v>25.44409872933333</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1608.56998527</v>
+      </c>
+      <c r="G18" t="n">
+        <v>22.774044308</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1585.795940964</v>
+      </c>
+      <c r="I18" t="n">
+        <v>26.68560294533333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4312.789545273999</v>
+      </c>
+      <c r="C19" t="n">
+        <v>36.30853267600001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4276.481012597999</v>
+      </c>
+      <c r="E19" t="n">
+        <v>25.30718837866667</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1696.902866872</v>
+      </c>
+      <c r="G19" t="n">
+        <v>22.475940104</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1674.426926766</v>
+      </c>
+      <c r="I19" t="n">
+        <v>26.55429984466667</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4427.371668214</v>
+      </c>
+      <c r="C20" t="n">
+        <v>35.672811882</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4391.698856334</v>
+      </c>
+      <c r="E20" t="n">
+        <v>25.31023158866667</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1708.110787172</v>
+      </c>
+      <c r="G20" t="n">
+        <v>22.116897024</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1685.993890148</v>
+      </c>
+      <c r="I20" t="n">
+        <v>26.56685283933334</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4719.73852585</v>
+      </c>
+      <c r="C21" t="n">
+        <v>35.270357802</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4684.468168048</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25.32196972466667</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1798.145568474</v>
+      </c>
+      <c r="G21" t="n">
+        <v>21.926013394</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1776.21955508</v>
+      </c>
+      <c r="I21" t="n">
+        <v>26.58711745933334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>